<commit_message>
updated piezo and sd
</commit_message>
<xml_diff>
--- a/SwitchBox/BOM for SwitchBox.xlsx
+++ b/SwitchBox/BOM for SwitchBox.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9084"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9084" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Index</t>
   </si>
@@ -90,12 +90,18 @@
   </si>
   <si>
     <t>Rubber Grommet</t>
+  </si>
+  <si>
+    <t>MicroSD Module</t>
+  </si>
+  <si>
+    <t>Piezo Buzzer</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -440,11 +446,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -609,7 +615,7 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D13" t="s">
         <v>20</v>
@@ -624,6 +630,28 @@
       </c>
       <c r="D14" t="s">
         <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="D15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="D16" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>